<commit_message>
updates on work sampling excel form parser
</commit_message>
<xml_diff>
--- a/cmi/core/utils/labor_records.xlsx
+++ b/cmi/core/utils/labor_records.xlsx
@@ -4,7 +4,7 @@
   <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet r:id="rId1" sheetId="1" name="labour"/>
@@ -568,7 +568,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -599,6 +599,12 @@
       <family val="2"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
       <b/>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -610,12 +616,6 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
@@ -1535,7 +1535,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="176">
+  <cellXfs count="175">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1591,169 +1591,169 @@
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="5" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="1" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="1" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="1" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="6" applyBorder="1" fontId="8" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="6" applyBorder="1" fontId="8" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="9" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="7" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="8" applyBorder="1" fontId="4" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="8" applyBorder="1" fontId="4" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="9" applyBorder="1" fontId="4" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="10" applyBorder="1" fontId="4" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="11" applyBorder="1" fontId="4" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="12" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="4" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="4" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="13" applyBorder="1" fontId="4" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="5" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="4" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="4" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="14" applyBorder="1" fontId="4" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="15" applyBorder="1" fontId="4" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="5" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="16" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="17" applyBorder="1" fontId="4" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="18" applyBorder="1" fontId="4" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="4" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="19" applyBorder="1" fontId="4" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="20" applyBorder="1" fontId="4" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="21" applyBorder="1" fontId="4" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="20" applyBorder="1" fontId="4" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="22" applyBorder="1" fontId="4" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="12" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="4" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="12" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="23" applyBorder="1" fontId="4" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="16" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="24" applyBorder="1" fontId="4" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="24" applyBorder="1" fontId="4" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="25" applyBorder="1" fontId="4" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="5" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="1" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="1" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="1" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="6" applyBorder="1" fontId="7" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="6" applyBorder="1" fontId="7" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="8" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="7" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="8" applyBorder="1" fontId="4" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="8" applyBorder="1" fontId="4" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="9" applyBorder="1" fontId="4" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="10" applyBorder="1" fontId="4" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="11" applyBorder="1" fontId="4" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="12" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="4" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="4" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="13" applyBorder="1" fontId="4" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="5" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="4" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="4" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="14" applyBorder="1" fontId="4" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="15" applyBorder="1" fontId="4" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="5" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="16" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="17" applyBorder="1" fontId="4" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="18" applyBorder="1" fontId="4" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="4" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="19" applyBorder="1" fontId="4" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="20" applyBorder="1" fontId="4" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="21" applyBorder="1" fontId="4" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="20" applyBorder="1" fontId="4" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="22" applyBorder="1" fontId="4" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="12" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="4" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="12" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="23" applyBorder="1" fontId="4" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="16" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="24" applyBorder="1" fontId="4" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="24" applyBorder="1" fontId="4" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="25" applyBorder="1" fontId="4" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="26" applyBorder="1" fontId="9" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="26" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="27" applyBorder="1" fontId="9" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="27" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="28" applyBorder="1" fontId="9" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="28" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="29" applyBorder="1" fontId="9" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="29" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="28" applyBorder="1" fontId="10" applyFont="1" fillId="0" applyAlignment="1">
@@ -1768,10 +1768,10 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="11" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="31" applyBorder="1" fontId="9" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="31" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="32" applyBorder="1" fontId="9" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="32" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="28" applyBorder="1" fontId="10" applyFont="1" fillId="0" applyAlignment="1">
@@ -1780,10 +1780,10 @@
     <xf xfId="0" numFmtId="0" borderId="29" applyBorder="1" fontId="10" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="33" applyBorder="1" fontId="9" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="33" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="34" applyBorder="1" fontId="9" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="34" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="35" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
@@ -1795,10 +1795,10 @@
     <xf xfId="0" numFmtId="0" borderId="29" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="7" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="8" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="36" applyBorder="1" fontId="7" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="36" applyBorder="1" fontId="8" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="5" applyBorder="1" fontId="4" applyFont="1" fillId="6" applyFill="1" applyAlignment="1">
@@ -1816,7 +1816,7 @@
     <xf xfId="0" numFmtId="0" borderId="7" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="37" applyBorder="1" fontId="7" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="37" applyBorder="1" fontId="8" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="38" applyBorder="1" fontId="12" applyFont="1" fillId="6" applyFill="1" applyAlignment="1">
@@ -1834,7 +1834,7 @@
     <xf xfId="0" numFmtId="15" applyNumberFormat="1" borderId="12" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="40" applyBorder="1" fontId="7" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="40" applyBorder="1" fontId="8" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="41" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
@@ -1852,7 +1852,7 @@
     <xf xfId="0" numFmtId="0" borderId="7" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="45" applyBorder="1" fontId="7" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="45" applyBorder="1" fontId="8" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="46" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
@@ -1894,7 +1894,7 @@
     <xf xfId="0" numFmtId="15" applyNumberFormat="1" borderId="16" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="52" applyBorder="1" fontId="7" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="52" applyBorder="1" fontId="8" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="53" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
@@ -1921,12 +1921,12 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="54" applyBorder="1" fontId="11" applyFont="1" fillId="7" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="13" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1954,15 +1954,15 @@
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
@@ -1984,15 +1984,12 @@
     <xf xfId="0" numFmtId="0" borderId="44" applyBorder="1" fontId="11" applyFont="1" fillId="8" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="38" applyBorder="1" fontId="11" applyFont="1" fillId="9" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="38" applyBorder="1" fontId="11" applyFont="1" fillId="9" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="38" applyBorder="1" fontId="11" applyFont="1" fillId="9" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="38" applyBorder="1" fontId="11" applyFont="1" fillId="9" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf xfId="0" numFmtId="0" borderId="38" applyBorder="1" fontId="11" applyFont="1" fillId="9" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -2044,13 +2041,13 @@
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="59" applyBorder="1" fontId="11" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="11" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="11" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="11" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="11" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="11" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -2366,12 +2363,12 @@
   </sheetPr>
   <dimension ref="A1:R12"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="68" width="8.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="173" width="11.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="69" width="8.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="172" width="11.290714285714287" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="69" width="9.576428571428572" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="68" width="11.290714285714287" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="69" width="10.719285714285713" customWidth="1" bestFit="1"/>
@@ -2383,17 +2380,17 @@
     <col min="11" max="11" style="69" width="14.290714285714287" customWidth="1" bestFit="1"/>
     <col min="12" max="12" style="69" width="15.290714285714287" customWidth="1" bestFit="1"/>
     <col min="13" max="13" style="69" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="174" width="14.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="173" width="14.290714285714287" customWidth="1" bestFit="1"/>
     <col min="15" max="15" style="68" width="11.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="175" width="11.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="175" width="17.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="174" width="11.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="17" max="17" style="174" width="17.576428571428572" customWidth="1" bestFit="1"/>
     <col min="18" max="18" style="68" width="11.290714285714287" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
-      <c r="A1" s="19"/>
-      <c r="B1" s="129"/>
-      <c r="C1" s="130"/>
+      <c r="A1" s="129"/>
+      <c r="B1" s="130"/>
+      <c r="C1" s="129"/>
       <c r="D1" s="19"/>
       <c r="E1" s="4"/>
       <c r="F1" s="131" t="s">
@@ -2413,9 +2410,9 @@
       <c r="R1" s="125"/>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
-      <c r="A2" s="19"/>
-      <c r="B2" s="129"/>
-      <c r="C2" s="130"/>
+      <c r="A2" s="129"/>
+      <c r="B2" s="130"/>
+      <c r="C2" s="129"/>
       <c r="D2" s="19"/>
       <c r="E2" s="4"/>
       <c r="F2" s="131" t="s">
@@ -2435,9 +2432,9 @@
       <c r="R2" s="125"/>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="19"/>
-      <c r="B3" s="129"/>
-      <c r="C3" s="130"/>
+      <c r="A3" s="129"/>
+      <c r="B3" s="130"/>
+      <c r="C3" s="129"/>
       <c r="D3" s="19"/>
       <c r="E3" s="4"/>
       <c r="F3" s="131" t="s">
@@ -2457,9 +2454,9 @@
       <c r="R3" s="19"/>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
-      <c r="A4" s="19"/>
-      <c r="B4" s="129"/>
-      <c r="C4" s="130"/>
+      <c r="A4" s="129"/>
+      <c r="B4" s="130"/>
+      <c r="C4" s="129"/>
       <c r="D4" s="19"/>
       <c r="E4" s="4"/>
       <c r="F4" s="134"/>
@@ -2479,9 +2476,9 @@
       <c r="R4" s="19"/>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
-      <c r="A5" s="19"/>
-      <c r="B5" s="129"/>
-      <c r="C5" s="130"/>
+      <c r="A5" s="129"/>
+      <c r="B5" s="130"/>
+      <c r="C5" s="129"/>
       <c r="D5" s="19"/>
       <c r="E5" s="4"/>
       <c r="F5" s="19"/>
@@ -2501,14 +2498,14 @@
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="29.625" customFormat="1" s="9">
       <c r="A6" s="140"/>
       <c r="B6" s="141"/>
-      <c r="C6" s="142"/>
-      <c r="D6" s="140"/>
+      <c r="C6" s="140"/>
+      <c r="D6" s="142"/>
       <c r="E6" s="143"/>
-      <c r="F6" s="140"/>
-      <c r="G6" s="140"/>
-      <c r="H6" s="140"/>
+      <c r="F6" s="142"/>
+      <c r="G6" s="142"/>
+      <c r="H6" s="142"/>
       <c r="I6" s="143"/>
-      <c r="J6" s="140"/>
+      <c r="J6" s="142"/>
       <c r="K6" s="144" t="s">
         <v>135</v>
       </c>
@@ -2537,226 +2534,226 @@
       <c r="B7" s="151" t="s">
         <v>142</v>
       </c>
-      <c r="C7" s="152" t="s">
+      <c r="C7" s="150" t="s">
         <v>143</v>
       </c>
-      <c r="D7" s="153" t="s">
+      <c r="D7" s="152" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="154" t="s">
+      <c r="E7" s="153" t="s">
         <v>144</v>
       </c>
-      <c r="F7" s="155" t="s">
+      <c r="F7" s="154" t="s">
         <v>145</v>
       </c>
-      <c r="G7" s="156" t="s">
+      <c r="G7" s="155" t="s">
         <v>146</v>
       </c>
-      <c r="H7" s="156" t="s">
+      <c r="H7" s="155" t="s">
         <v>147</v>
       </c>
-      <c r="I7" s="157" t="s">
+      <c r="I7" s="156" t="s">
         <v>148</v>
       </c>
-      <c r="J7" s="156" t="s">
+      <c r="J7" s="155" t="s">
         <v>149</v>
       </c>
-      <c r="K7" s="158" t="s">
+      <c r="K7" s="157" t="s">
         <v>150</v>
       </c>
-      <c r="L7" s="158" t="s">
+      <c r="L7" s="157" t="s">
         <v>151</v>
       </c>
-      <c r="M7" s="158" t="s">
+      <c r="M7" s="157" t="s">
         <v>152</v>
       </c>
-      <c r="N7" s="158"/>
-      <c r="O7" s="159"/>
-      <c r="P7" s="160"/>
-      <c r="Q7" s="161" t="s">
+      <c r="N7" s="157"/>
+      <c r="O7" s="158"/>
+      <c r="P7" s="159"/>
+      <c r="Q7" s="160" t="s">
         <v>153</v>
       </c>
-      <c r="R7" s="162"/>
+      <c r="R7" s="161"/>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="45">
-      <c r="A8" s="163">
+      <c r="A8" s="162">
         <v>1</v>
       </c>
-      <c r="B8" s="164">
+      <c r="B8" s="163">
         <v>42827</v>
       </c>
-      <c r="C8" s="163" t="s">
+      <c r="C8" s="162" t="s">
         <v>154</v>
       </c>
-      <c r="D8" s="165" t="s">
+      <c r="D8" s="164" t="s">
         <v>155</v>
       </c>
-      <c r="E8" s="166">
+      <c r="E8" s="165">
         <v>2</v>
       </c>
-      <c r="F8" s="167" t="s">
+      <c r="F8" s="166" t="s">
         <v>156</v>
       </c>
-      <c r="G8" s="165" t="s">
+      <c r="G8" s="164" t="s">
         <v>157</v>
       </c>
-      <c r="H8" s="167"/>
-      <c r="I8" s="168">
+      <c r="H8" s="166"/>
+      <c r="I8" s="167">
         <v>11</v>
       </c>
-      <c r="J8" s="167" t="s">
+      <c r="J8" s="166" t="s">
         <v>158</v>
       </c>
-      <c r="K8" s="168">
+      <c r="K8" s="167">
         <v>8</v>
       </c>
-      <c r="L8" s="168">
+      <c r="L8" s="167">
         <v>0</v>
       </c>
-      <c r="M8" s="168">
+      <c r="M8" s="167">
         <v>8</v>
       </c>
-      <c r="N8" s="168">
+      <c r="N8" s="167">
         <f>I8*K8</f>
       </c>
-      <c r="O8" s="167" t="s">
+      <c r="O8" s="166" t="s">
         <v>159</v>
       </c>
-      <c r="P8" s="169">
+      <c r="P8" s="168">
         <v>35.043</v>
       </c>
-      <c r="Q8" s="169">
+      <c r="Q8" s="168">
         <f>P8/N8</f>
       </c>
-      <c r="R8" s="167" t="s">
+      <c r="R8" s="166" t="s">
         <v>160</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="44.25">
-      <c r="A9" s="163">
+      <c r="A9" s="162">
         <v>2</v>
       </c>
-      <c r="B9" s="164">
+      <c r="B9" s="163">
         <v>42827</v>
       </c>
-      <c r="C9" s="163">
+      <c r="C9" s="162">
         <v>2</v>
       </c>
-      <c r="D9" s="165" t="s">
+      <c r="D9" s="164" t="s">
         <v>155</v>
       </c>
-      <c r="E9" s="166">
+      <c r="E9" s="165">
         <v>2</v>
       </c>
-      <c r="F9" s="167" t="s">
+      <c r="F9" s="166" t="s">
         <v>156</v>
       </c>
-      <c r="G9" s="165" t="s">
+      <c r="G9" s="164" t="s">
         <v>157</v>
       </c>
-      <c r="H9" s="167"/>
-      <c r="I9" s="168">
+      <c r="H9" s="166"/>
+      <c r="I9" s="167">
         <v>11</v>
       </c>
-      <c r="J9" s="167" t="s">
+      <c r="J9" s="166" t="s">
         <v>158</v>
       </c>
-      <c r="K9" s="168">
+      <c r="K9" s="167">
         <v>8</v>
       </c>
-      <c r="L9" s="168">
+      <c r="L9" s="167">
         <v>0</v>
       </c>
-      <c r="M9" s="168">
+      <c r="M9" s="167">
         <v>8</v>
       </c>
-      <c r="N9" s="168">
+      <c r="N9" s="167">
         <f>I9*K9</f>
       </c>
-      <c r="O9" s="167" t="s">
+      <c r="O9" s="166" t="s">
         <v>159</v>
       </c>
-      <c r="P9" s="169">
+      <c r="P9" s="168">
         <v>35.043</v>
       </c>
-      <c r="Q9" s="169">
+      <c r="Q9" s="168">
         <f>P9/N9</f>
       </c>
-      <c r="R9" s="167" t="s">
+      <c r="R9" s="166" t="s">
         <v>160</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
-      <c r="A10" s="170"/>
-      <c r="B10" s="171"/>
-      <c r="C10" s="172"/>
-      <c r="D10" s="170"/>
-      <c r="E10" s="172"/>
-      <c r="F10" s="170"/>
-      <c r="G10" s="170"/>
-      <c r="H10" s="170"/>
-      <c r="I10" s="172"/>
-      <c r="J10" s="170"/>
-      <c r="K10" s="172"/>
-      <c r="L10" s="172"/>
-      <c r="M10" s="172"/>
-      <c r="N10" s="168">
+      <c r="A10" s="169"/>
+      <c r="B10" s="170"/>
+      <c r="C10" s="169"/>
+      <c r="D10" s="171"/>
+      <c r="E10" s="169"/>
+      <c r="F10" s="171"/>
+      <c r="G10" s="171"/>
+      <c r="H10" s="171"/>
+      <c r="I10" s="169"/>
+      <c r="J10" s="171"/>
+      <c r="K10" s="169"/>
+      <c r="L10" s="169"/>
+      <c r="M10" s="169"/>
+      <c r="N10" s="167">
         <f>I10*K10</f>
       </c>
-      <c r="O10" s="170"/>
-      <c r="P10" s="169"/>
-      <c r="Q10" s="169">
+      <c r="O10" s="171"/>
+      <c r="P10" s="168"/>
+      <c r="Q10" s="168">
         <f>P10/N10</f>
       </c>
-      <c r="R10" s="170"/>
+      <c r="R10" s="171"/>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
-      <c r="A11" s="170"/>
-      <c r="B11" s="171"/>
-      <c r="C11" s="172"/>
-      <c r="D11" s="170"/>
-      <c r="E11" s="172"/>
-      <c r="F11" s="170"/>
-      <c r="G11" s="170"/>
-      <c r="H11" s="170"/>
-      <c r="I11" s="172"/>
-      <c r="J11" s="170"/>
-      <c r="K11" s="172"/>
-      <c r="L11" s="172"/>
-      <c r="M11" s="172"/>
-      <c r="N11" s="168">
+      <c r="A11" s="169"/>
+      <c r="B11" s="170"/>
+      <c r="C11" s="169"/>
+      <c r="D11" s="171"/>
+      <c r="E11" s="169"/>
+      <c r="F11" s="171"/>
+      <c r="G11" s="171"/>
+      <c r="H11" s="171"/>
+      <c r="I11" s="169"/>
+      <c r="J11" s="171"/>
+      <c r="K11" s="169"/>
+      <c r="L11" s="169"/>
+      <c r="M11" s="169"/>
+      <c r="N11" s="167">
         <f>I11*K11</f>
       </c>
-      <c r="O11" s="170"/>
-      <c r="P11" s="169"/>
-      <c r="Q11" s="169">
+      <c r="O11" s="171"/>
+      <c r="P11" s="168"/>
+      <c r="Q11" s="168">
         <f>P11/N11</f>
       </c>
-      <c r="R11" s="170"/>
+      <c r="R11" s="171"/>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
-      <c r="A12" s="170"/>
-      <c r="B12" s="171"/>
-      <c r="C12" s="172"/>
-      <c r="D12" s="170"/>
-      <c r="E12" s="172"/>
-      <c r="F12" s="170"/>
-      <c r="G12" s="170"/>
-      <c r="H12" s="170"/>
-      <c r="I12" s="172"/>
-      <c r="J12" s="170"/>
-      <c r="K12" s="172"/>
-      <c r="L12" s="172"/>
-      <c r="M12" s="172"/>
-      <c r="N12" s="168">
+      <c r="A12" s="169"/>
+      <c r="B12" s="170"/>
+      <c r="C12" s="169"/>
+      <c r="D12" s="171"/>
+      <c r="E12" s="169"/>
+      <c r="F12" s="171"/>
+      <c r="G12" s="171"/>
+      <c r="H12" s="171"/>
+      <c r="I12" s="169"/>
+      <c r="J12" s="171"/>
+      <c r="K12" s="169"/>
+      <c r="L12" s="169"/>
+      <c r="M12" s="169"/>
+      <c r="N12" s="167">
         <f>I12*K12</f>
       </c>
-      <c r="O12" s="170"/>
-      <c r="P12" s="169"/>
-      <c r="Q12" s="169">
+      <c r="O12" s="171"/>
+      <c r="P12" s="168"/>
+      <c r="Q12" s="168">
         <f>P12/N12</f>
       </c>
-      <c r="R12" s="170"/>
+      <c r="R12" s="171"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -2780,7 +2777,7 @@
   </sheetPr>
   <dimension ref="A1:AO104"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3105,7 +3102,7 @@
       <c r="AN6" s="77"/>
       <c r="AO6" s="77"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="19"/>
       <c r="B7" s="82"/>
       <c r="C7" s="83"/>
@@ -3152,7 +3149,7 @@
       <c r="AN7" s="77"/>
       <c r="AO7" s="77"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="20.25">
       <c r="A8" s="19"/>
       <c r="B8" s="19"/>
       <c r="C8" s="19"/>
@@ -3195,7 +3192,7 @@
       <c r="AN8" s="4"/>
       <c r="AO8" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="20.25">
       <c r="A9" s="84" t="s">
         <v>111</v>
       </c>
@@ -3206,7 +3203,7 @@
       </c>
       <c r="E9" s="88"/>
       <c r="F9" s="89">
-        <v>2.082962962962963</v>
+        <v>3.082777777777778</v>
       </c>
       <c r="G9" s="90"/>
       <c r="H9" s="90"/>
@@ -3244,7 +3241,7 @@
       <c r="AN9" s="90"/>
       <c r="AO9" s="91"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="22.5">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="20.25">
       <c r="A10" s="92" t="s">
         <v>113</v>
       </c>
@@ -3365,7 +3362,7 @@
         <v>18</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="20.25">
       <c r="A11" s="92" t="s">
         <v>116</v>
       </c>
@@ -3412,7 +3409,7 @@
       <c r="AN11" s="96"/>
       <c r="AO11" s="97"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="14.25">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
       <c r="A12" s="92" t="s">
         <v>118</v>
       </c>
@@ -3461,7 +3458,7 @@
       <c r="AN12" s="103"/>
       <c r="AO12" s="104"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="15">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
       <c r="A13" s="105" t="s">
         <v>121</v>
       </c>
@@ -3508,7 +3505,7 @@
       <c r="AN13" s="109"/>
       <c r="AO13" s="110"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="14.25">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
       <c r="A14" s="111"/>
       <c r="B14" s="111"/>
       <c r="C14" s="99"/>
@@ -3553,7 +3550,7 @@
       <c r="AN14" s="109"/>
       <c r="AO14" s="110"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="14.25">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
       <c r="A15" s="112" t="s">
         <v>124</v>
       </c>
@@ -3600,7 +3597,7 @@
       <c r="AN15" s="109"/>
       <c r="AO15" s="110"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="14.25">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
       <c r="A16" s="113"/>
       <c r="B16" s="114"/>
       <c r="C16" s="99"/>
@@ -3645,7 +3642,7 @@
       <c r="AN16" s="109"/>
       <c r="AO16" s="110"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="15">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
       <c r="A17" s="113"/>
       <c r="B17" s="114"/>
       <c r="C17" s="99"/>
@@ -3690,7 +3687,7 @@
       <c r="AN17" s="109"/>
       <c r="AO17" s="110"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
       <c r="A18" s="113"/>
       <c r="B18" s="114"/>
       <c r="C18" s="99"/>
@@ -3735,7 +3732,7 @@
       <c r="AN18" s="116"/>
       <c r="AO18" s="117"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
       <c r="A19" s="118"/>
       <c r="B19" s="111"/>
       <c r="C19" s="119"/>
@@ -3852,7 +3849,7 @@
         <f>SUM(AO12:AO18)</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="20.25">
       <c r="A20" s="19"/>
       <c r="B20" s="19"/>
       <c r="C20" s="19"/>
@@ -3895,7 +3892,7 @@
       <c r="AN20" s="4"/>
       <c r="AO20" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="20.25">
       <c r="A21" s="125" t="s">
         <v>5</v>
       </c>
@@ -3944,7 +3941,7 @@
       <c r="AN21" s="90"/>
       <c r="AO21" s="91"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="20.25">
       <c r="A22" s="19"/>
       <c r="B22" s="19"/>
       <c r="C22" s="19"/>
@@ -4061,7 +4058,7 @@
         <v>18</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="20.25">
       <c r="A23" s="19"/>
       <c r="B23" s="19"/>
       <c r="C23" s="19"/>
@@ -4592,7 +4589,7 @@
       </c>
       <c r="E33" s="88"/>
       <c r="F33" s="89">
-        <v>2.1662962962962964</v>
+        <v>3.1661111111111113</v>
       </c>
       <c r="G33" s="90"/>
       <c r="H33" s="90"/>
@@ -5278,7 +5275,7 @@
       </c>
       <c r="E45" s="88"/>
       <c r="F45" s="89">
-        <v>2.207962962962963</v>
+        <v>3.207777777777778</v>
       </c>
       <c r="G45" s="90"/>
       <c r="H45" s="90"/>
@@ -5964,7 +5961,7 @@
       </c>
       <c r="E57" s="88"/>
       <c r="F57" s="89">
-        <v>2.7912962962962964</v>
+        <v>3.7911111111111113</v>
       </c>
       <c r="G57" s="90"/>
       <c r="H57" s="90"/>
@@ -6650,7 +6647,7 @@
       </c>
       <c r="E69" s="88"/>
       <c r="F69" s="89">
-        <v>2.832962962962963</v>
+        <v>3.832777777777778</v>
       </c>
       <c r="G69" s="90"/>
       <c r="H69" s="90"/>
@@ -7336,7 +7333,7 @@
       </c>
       <c r="E81" s="88"/>
       <c r="F81" s="89">
-        <v>2.87462962962963</v>
+        <v>3.8744444444444444</v>
       </c>
       <c r="G81" s="90"/>
       <c r="H81" s="90"/>
@@ -8022,7 +8019,7 @@
       </c>
       <c r="E93" s="88"/>
       <c r="F93" s="89">
-        <v>2.9162962962962964</v>
+        <v>3.9161111111111113</v>
       </c>
       <c r="G93" s="90"/>
       <c r="H93" s="90"/>

</xml_diff>